<commit_message>
Finalize fast close slow far strategy
</commit_message>
<xml_diff>
--- a/src/strategy/fast-close-slow-far/paths-by-ceacon-power.xlsx
+++ b/src/strategy/fast-close-slow-far/paths-by-ceacon-power.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moi\Documents\Dev\Codingame\codinggamespringchallenge2023\src\strategy\fast-close-slow-far\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88140F56-0F28-41AA-A073-2074081CBD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8BE6D4-5B5E-432D-9098-B70E2AE3F405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="3015" windowWidth="19140" windowHeight="11220" activeTab="2" xr2:uid="{51EAAA72-26A2-48C7-B87B-564FC0557B48}"/>
+    <workbookView xWindow="6790" yWindow="16930" windowWidth="19140" windowHeight="11220" activeTab="3" xr2:uid="{51EAAA72-26A2-48C7-B87B-564FC0557B48}"/>
   </bookViews>
   <sheets>
     <sheet name="initial state" sheetId="1" r:id="rId1"/>
     <sheet name="closest" sheetId="2" r:id="rId2"/>
     <sheet name="closest with more crystals" sheetId="3" r:id="rId3"/>
+    <sheet name="test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Beacon power shortest path</t>
   </si>
@@ -901,7 +902,7 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
         <v>10.24390243902439</v>
       </c>
@@ -922,7 +923,7 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="3">
         <f t="shared" si="1"/>
         <v>10.434782608695652</v>
       </c>
@@ -987,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02041BF1-7977-4128-9FE3-74B57F8276E3}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1111,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="1">
         <f t="shared" si="1"/>
         <v>9.2307692307692299</v>
       </c>
@@ -1173,7 +1174,7 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
         <v>10.24390243902439</v>
       </c>
@@ -1194,7 +1195,7 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="3">
         <f t="shared" si="1"/>
         <v>10.434782608695652</v>
       </c>
@@ -1243,6 +1244,277 @@
       <c r="D13" s="3">
         <f t="shared" si="2"/>
         <v>1.0714285714285714</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AC337B-8886-46C7-9198-AFC36C7B8E9F}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>($B$2*$A4)+$C$2</f>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <f>($A$2/$B4)*$A4</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="D4" s="1">
+        <f>($A$2/$B4)</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="E4">
+        <f>$B$2*$C4+$D4*$C$2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B13" si="0">($B$2*$A5)+$C$2</f>
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" ref="C5:C13" si="1">($A$2/$B5)*$A5</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:D13" si="2">($A$2/$B5)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E13" si="3">$B$2*$C5+$D5*$C$2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>16.363636363636363</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="2"/>
+        <v>5.4545454545454541</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="1"/>
+        <v>18.46153846153846</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="2"/>
+        <v>4.615384615384615</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>59.999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>21.176470588235293</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5294117647058822</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>22.105263157894736</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1578947368421053</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="1"/>
+        <v>22.857142857142858</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="1"/>
+        <v>23.478260869565219</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6086956521739131</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="3"/>

</xml_diff>